<commit_message>
Save Work in Progress
</commit_message>
<xml_diff>
--- a/Adv.Tools.UI/Resources/DefaultSettings.xlsx
+++ b/Adv.Tools.UI/Resources/DefaultSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\source\repos\Adv.Tools\Adv.Tools.UI\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFFE28B-EC74-408A-B783-DA84EA2AC6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492870AA-50C3-42A0-B458-11FBB09A9369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="2670" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpectedSharedPara" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="146">
   <si>
     <t>PARAMETER</t>
   </si>
@@ -34,36 +34,6 @@
     <t>GUID</t>
   </si>
   <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>DATATYPE</t>
-  </si>
-  <si>
-    <t>DATACATEGORY</t>
-  </si>
-  <si>
-    <t>GROUP</t>
-  </si>
-  <si>
-    <t>VISIBLE</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>USERMODIFIABLE</t>
-  </si>
-  <si>
-    <t>HIDEWHENNOVALUE</t>
-  </si>
-  <si>
-    <t>PARAM</t>
-  </si>
-  <si>
-    <t>TEXT</t>
-  </si>
-  <si>
     <t>f7a6077e-5e78-48b2-9679-cfa260d36fa5</t>
   </si>
   <si>
@@ -100,9 +70,6 @@
     <t>ADV_Scale</t>
   </si>
   <si>
-    <t>INTEGER</t>
-  </si>
-  <si>
     <t>e573297a-ebee-4ef6-9fcb-a6cf56a46061</t>
   </si>
   <si>
@@ -430,9 +397,6 @@
     <t>ADV_Open_Height</t>
   </si>
   <si>
-    <t>LENGTH</t>
-  </si>
-  <si>
     <t>bbf8bf19-c8cb-4f25-a8ab-7c65826fe809</t>
   </si>
   <si>
@@ -443,9 +407,6 @@
   </si>
   <si>
     <t>ADV_Tender</t>
-  </si>
-  <si>
-    <t>YESNO</t>
   </si>
   <si>
     <t>8ca8d21f-1b36-4ba0-bc1c-3e6f0130eb43</t>
@@ -1343,464 +1304,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>135</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B14" t="s">
         <v>136</v>
       </c>
-      <c r="D4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
         <v>11</v>
       </c>
-      <c r="F15">
-        <v>4</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17">
-        <v>4</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E1C624-7D33-4737-AB85-12DEA8D1BEEB}">
   <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1825,29 +1475,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C3">
         <v>-2000220</v>
@@ -1855,10 +1505,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C4">
         <v>-2000240</v>
@@ -1866,10 +1516,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>-2006000</v>
@@ -1877,10 +1527,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>-2003400</v>
@@ -1888,10 +1538,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>-2000011</v>
@@ -1899,10 +1549,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>-2001330</v>
@@ -1910,10 +1560,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C9">
         <v>-2001320</v>
@@ -1921,10 +1571,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C10">
         <v>-2000032</v>
@@ -1932,10 +1582,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C11">
         <v>-2001360</v>
@@ -1943,10 +1593,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <v>-2001260</v>
@@ -1954,10 +1604,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C13">
         <v>-2001180</v>
@@ -1965,10 +1615,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C14">
         <v>-2001340</v>
@@ -1976,10 +1626,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C15">
         <v>-2001120</v>
@@ -1987,10 +1637,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C16">
         <v>-2001100</v>
@@ -1998,10 +1648,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C17">
         <v>-2000080</v>
@@ -2009,10 +1659,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C18">
         <v>-2000038</v>
@@ -2020,10 +1670,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C19">
         <v>-2000032</v>
@@ -2031,10 +1681,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>-2001352</v>
@@ -2042,10 +1692,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>-2001352</v>
@@ -2053,10 +1703,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>-2001352</v>
@@ -2064,10 +1714,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>-2001352</v>
@@ -2075,10 +1725,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>-2001352</v>
@@ -2086,10 +1736,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>-2001352</v>
@@ -2097,10 +1747,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>-2001352</v>
@@ -2108,10 +1758,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C27">
         <v>-2001352</v>
@@ -2119,18 +1769,18 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C29">
         <v>-2000220</v>
@@ -2138,10 +1788,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C30">
         <v>-2000240</v>
@@ -2149,10 +1799,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>-2006000</v>
@@ -2160,10 +1810,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>-2001300</v>
@@ -2171,10 +1821,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C33">
         <v>-2000032</v>
@@ -2182,10 +1832,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C34">
         <v>-2000011</v>
@@ -2193,10 +1843,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C35">
         <v>-2001330</v>
@@ -2204,10 +1854,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <v>-2001320</v>
@@ -2215,10 +1865,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>-2000120</v>
@@ -2226,10 +1876,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C38">
         <v>-2001336</v>
@@ -2237,10 +1887,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C39">
         <v>-2009000</v>
@@ -2248,10 +1898,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C40">
         <v>-2009060</v>
@@ -2259,10 +1909,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>-2001352</v>
@@ -2270,10 +1920,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C42">
         <v>-2001352</v>
@@ -2281,10 +1931,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C43">
         <v>-2001352</v>
@@ -2292,10 +1942,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C44">
         <v>-2001352</v>
@@ -2303,10 +1953,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
         <v>31</v>
-      </c>
-      <c r="B45" t="s">
-        <v>42</v>
       </c>
       <c r="C45">
         <v>-2001352</v>
@@ -2314,10 +1964,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C46">
         <v>-2001352</v>
@@ -2325,10 +1975,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C47">
         <v>-2001352</v>
@@ -2336,10 +1986,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C48">
         <v>-2001352</v>
@@ -2347,18 +1997,18 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C50">
         <v>-2000240</v>
@@ -2366,10 +2016,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C51">
         <v>-2000220</v>
@@ -2377,10 +2027,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C52">
         <v>-2006000</v>
@@ -2388,10 +2038,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C53">
         <v>-2001040</v>
@@ -2399,10 +2049,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C54">
         <v>-2001043</v>
@@ -2410,10 +2060,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C55">
         <v>-2001140</v>
@@ -2421,10 +2071,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C56">
         <v>-2000985</v>
@@ -2432,10 +2082,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C57">
         <v>-2001046</v>
@@ -2443,10 +2093,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C58">
         <v>-2008234</v>
@@ -2454,10 +2104,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C59">
         <v>-2001350</v>
@@ -2465,10 +2115,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C60">
         <v>-2001010</v>
@@ -2476,10 +2126,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C61">
         <v>-2001055</v>
@@ -2487,10 +2137,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C62">
         <v>-2008081</v>
@@ -2498,10 +2148,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C63">
         <v>-2008083</v>
@@ -2509,10 +2159,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C64">
         <v>-2008232</v>
@@ -2520,10 +2170,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C65">
         <v>-2008079</v>
@@ -2531,10 +2181,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C66">
         <v>-2008075</v>
@@ -2542,10 +2192,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C67">
         <v>-2001060</v>
@@ -2553,10 +2203,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" t="s">
         <v>46</v>
-      </c>
-      <c r="B68" t="s">
-        <v>57</v>
       </c>
       <c r="C68">
         <v>-2008050</v>
@@ -2564,10 +2214,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" t="s">
         <v>46</v>
-      </c>
-      <c r="B69" t="s">
-        <v>57</v>
       </c>
       <c r="C69">
         <v>-2008208</v>
@@ -2575,10 +2225,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" t="s">
         <v>46</v>
-      </c>
-      <c r="B70" t="s">
-        <v>57</v>
       </c>
       <c r="C70">
         <v>-2008055</v>
@@ -2586,10 +2236,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" t="s">
         <v>46</v>
-      </c>
-      <c r="B71" t="s">
-        <v>57</v>
       </c>
       <c r="C71">
         <v>-2008049</v>
@@ -2597,10 +2247,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" t="s">
         <v>46</v>
-      </c>
-      <c r="B72" t="s">
-        <v>57</v>
       </c>
       <c r="C72">
         <v>-2008122</v>
@@ -2608,10 +2258,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" t="s">
         <v>46</v>
-      </c>
-      <c r="B73" t="s">
-        <v>57</v>
       </c>
       <c r="C73">
         <v>-2008161</v>
@@ -2619,10 +2269,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" t="s">
         <v>46</v>
-      </c>
-      <c r="B74" t="s">
-        <v>57</v>
       </c>
       <c r="C74">
         <v>-2008044</v>
@@ -2630,10 +2280,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C75">
         <v>-2008000</v>
@@ -2641,10 +2291,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C76">
         <v>-2008020</v>
@@ -2652,10 +2302,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B77" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C77">
         <v>-2008013</v>
@@ -2663,10 +2313,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C78">
         <v>-2001352</v>
@@ -2674,10 +2324,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B79" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C79">
         <v>-2001352</v>
@@ -2685,10 +2335,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B80" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C80">
         <v>-2001352</v>
@@ -2696,10 +2346,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B81" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C81">
         <v>-2001352</v>
@@ -2707,10 +2357,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B82" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C82">
         <v>-2001352</v>
@@ -2718,10 +2368,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B83" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C83">
         <v>-2001352</v>
@@ -2729,10 +2379,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B84" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C84">
         <v>-2001352</v>
@@ -2740,10 +2390,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C85">
         <v>-2001352</v>
@@ -2751,18 +2401,18 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B87" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C87">
         <v>-2000220</v>
@@ -2770,10 +2420,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B88" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C88">
         <v>-2000240</v>
@@ -2781,10 +2431,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B89" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C89">
         <v>-2006000</v>
@@ -2792,10 +2442,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B90" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C90">
         <v>-2001040</v>
@@ -2803,10 +2453,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B91" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C91">
         <v>-2001043</v>
@@ -2814,10 +2464,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B92" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C92">
         <v>-2001140</v>
@@ -2825,10 +2475,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B93" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C93">
         <v>-2000985</v>
@@ -2836,10 +2486,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B94" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C94">
         <v>-2001046</v>
@@ -2847,10 +2497,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B95" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C95">
         <v>-2008234</v>
@@ -2858,10 +2508,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B96" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C96">
         <v>-2001350</v>
@@ -2869,10 +2519,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B97" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C97">
         <v>-2001010</v>
@@ -2880,10 +2530,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B98" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C98">
         <v>-2001055</v>
@@ -2891,10 +2541,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B99" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C99">
         <v>-2008081</v>
@@ -2902,10 +2552,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B100" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C100">
         <v>-2008083</v>
@@ -2913,10 +2563,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B101" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C101">
         <v>-2008232</v>
@@ -2924,10 +2574,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B102" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C102">
         <v>-2008079</v>
@@ -2935,10 +2585,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B103" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C103">
         <v>-2008075</v>
@@ -2946,10 +2596,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B104" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C104">
         <v>-2001060</v>
@@ -2957,10 +2607,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B105" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C105">
         <v>-2008050</v>
@@ -2968,10 +2618,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C106">
         <v>-2008208</v>
@@ -2979,10 +2629,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B107" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C107">
         <v>-2008055</v>
@@ -2990,10 +2640,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B108" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C108">
         <v>-2008049</v>
@@ -3001,10 +2651,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B109" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C109">
         <v>-2008122</v>
@@ -3012,10 +2662,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B110" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C110">
         <v>-2008161</v>
@@ -3023,10 +2673,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B111" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C111">
         <v>-2008044</v>
@@ -3034,10 +2684,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B112" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C112">
         <v>-2001352</v>
@@ -3045,10 +2695,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B113" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C113">
         <v>-2001352</v>
@@ -3056,10 +2706,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B114" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C114">
         <v>-2001352</v>
@@ -3067,10 +2717,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B115" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C115">
         <v>-2001352</v>
@@ -3078,10 +2728,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B116" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C116">
         <v>-2001352</v>
@@ -3089,10 +2739,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B117" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C117">
         <v>-2001352</v>
@@ -3100,10 +2750,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C118">
         <v>-2001352</v>
@@ -3111,10 +2761,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B119" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C119">
         <v>-2001352</v>
@@ -3122,18 +2772,18 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B120" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C121">
         <v>-2000240</v>
@@ -3141,10 +2791,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C122">
         <v>-2000220</v>
@@ -3152,10 +2802,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B123" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C123">
         <v>-2006000</v>
@@ -3163,10 +2813,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>67</v>
+      </c>
+      <c r="B124" t="s">
         <v>78</v>
-      </c>
-      <c r="B124" t="s">
-        <v>89</v>
       </c>
       <c r="C124">
         <v>-2001040</v>
@@ -3174,10 +2824,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>67</v>
+      </c>
+      <c r="B125" t="s">
         <v>78</v>
-      </c>
-      <c r="B125" t="s">
-        <v>89</v>
       </c>
       <c r="C125">
         <v>-2001043</v>
@@ -3185,10 +2835,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>67</v>
+      </c>
+      <c r="B126" t="s">
         <v>78</v>
-      </c>
-      <c r="B126" t="s">
-        <v>89</v>
       </c>
       <c r="C126">
         <v>-2001140</v>
@@ -3196,10 +2846,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>67</v>
+      </c>
+      <c r="B127" t="s">
         <v>78</v>
-      </c>
-      <c r="B127" t="s">
-        <v>89</v>
       </c>
       <c r="C127">
         <v>-2000985</v>
@@ -3207,10 +2857,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>67</v>
+      </c>
+      <c r="B128" t="s">
         <v>78</v>
-      </c>
-      <c r="B128" t="s">
-        <v>89</v>
       </c>
       <c r="C128">
         <v>-2001046</v>
@@ -3218,10 +2868,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>67</v>
+      </c>
+      <c r="B129" t="s">
         <v>78</v>
-      </c>
-      <c r="B129" t="s">
-        <v>89</v>
       </c>
       <c r="C129">
         <v>-2008234</v>
@@ -3229,10 +2879,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>67</v>
+      </c>
+      <c r="B130" t="s">
         <v>78</v>
-      </c>
-      <c r="B130" t="s">
-        <v>89</v>
       </c>
       <c r="C130">
         <v>-2001350</v>
@@ -3240,10 +2890,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>67</v>
+      </c>
+      <c r="B131" t="s">
         <v>78</v>
-      </c>
-      <c r="B131" t="s">
-        <v>89</v>
       </c>
       <c r="C131">
         <v>-2001010</v>
@@ -3251,10 +2901,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C132">
         <v>-2001055</v>
@@ -3262,10 +2912,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B133" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C133">
         <v>-2008081</v>
@@ -3273,10 +2923,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B134" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C134">
         <v>-2008083</v>
@@ -3284,10 +2934,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B135" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C135">
         <v>-2008232</v>
@@ -3295,10 +2945,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B136" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C136">
         <v>-2008079</v>
@@ -3306,10 +2956,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B137" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C137">
         <v>-2008075</v>
@@ -3317,10 +2967,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B138" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C138">
         <v>-2001060</v>
@@ -3328,10 +2978,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B139" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C139">
         <v>-2008126</v>
@@ -3339,10 +2989,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B140" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C140">
         <v>-2008150</v>
@@ -3350,10 +3000,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B141" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C141">
         <v>-2008130</v>
@@ -3361,10 +3011,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B142" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C142">
         <v>-2008128</v>
@@ -3372,10 +3022,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B143" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C143">
         <v>-2008149</v>
@@ -3383,10 +3033,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B144" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C144">
         <v>-2008132</v>
@@ -3394,10 +3044,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B145" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C145">
         <v>-2001120</v>
@@ -3405,10 +3055,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B146" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C146">
         <v>-2001352</v>
@@ -3416,10 +3066,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B147" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C147">
         <v>-2001352</v>
@@ -3427,10 +3077,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B148" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C148">
         <v>-2001352</v>
@@ -3438,10 +3088,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B149" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C149">
         <v>-2001352</v>
@@ -3449,10 +3099,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B150" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C150">
         <v>-2001352</v>
@@ -3460,10 +3110,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B151" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C151">
         <v>-2001352</v>
@@ -3471,10 +3121,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B152" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C152">
         <v>-2001352</v>
@@ -3482,10 +3132,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B153" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C153">
         <v>-2001352</v>
@@ -3493,10 +3143,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B154" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C154">
         <v>-2000220</v>
@@ -3504,10 +3154,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B155" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C155">
         <v>-2000240</v>
@@ -3515,18 +3165,18 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B156" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B157" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C157">
         <v>-2006000</v>
@@ -3534,10 +3184,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B158" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C158">
         <v>-2001260</v>
@@ -3545,10 +3195,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B159" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C159">
         <v>-2001180</v>
@@ -3556,10 +3206,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B160" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C160">
         <v>-2001340</v>
@@ -3567,10 +3217,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B161" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C161">
         <v>-2001360</v>
@@ -3578,10 +3228,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B162" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C162">
         <v>-2003400</v>
@@ -3589,10 +3239,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B163" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C163">
         <v>-2000032</v>
@@ -3600,10 +3250,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B164" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C164">
         <v>-2001352</v>
@@ -3611,10 +3261,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>85</v>
+      </c>
+      <c r="B165" t="s">
         <v>96</v>
-      </c>
-      <c r="B165" t="s">
-        <v>107</v>
       </c>
       <c r="C165">
         <v>-2001352</v>
@@ -3622,10 +3272,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B166" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C166">
         <v>-2001352</v>
@@ -3633,10 +3283,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B167" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C167">
         <v>-2001352</v>
@@ -3644,10 +3294,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B168" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C168">
         <v>-2001352</v>
@@ -3655,10 +3305,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B169" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C169">
         <v>-2001352</v>
@@ -3666,10 +3316,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B170" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C170">
         <v>-2001352</v>
@@ -3677,10 +3327,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B171" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C171">
         <v>-2001352</v>
@@ -3711,27 +3361,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3739,13 +3389,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3753,13 +3403,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3767,13 +3417,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3781,13 +3431,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3795,13 +3445,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3809,13 +3459,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
         <v>143</v>
-      </c>
-      <c r="C8" t="s">
-        <v>156</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3823,13 +3473,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3837,13 +3487,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3851,13 +3501,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3865,13 +3515,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -3879,13 +3529,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -3893,13 +3543,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -3907,13 +3557,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -3921,13 +3571,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -3935,13 +3585,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D17">
         <v>7</v>

</xml_diff>